<commit_message>
Updated E car properties and Comp Files
</commit_message>
<xml_diff>
--- a/2017_FSAEA_TRACK_DATA.xlsx
+++ b/2017_FSAEA_TRACK_DATA.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ambar-Surface\Downloads\Lap Sim 2017 10_11\Lap Sim 2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ambar\Documents\MUR\lapSim2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11438" windowHeight="5903" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11445" windowHeight="5910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -423,23 +423,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.59765625" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="18.265625" customWidth="1"/>
-    <col min="4" max="4" width="16.73046875" customWidth="1"/>
-    <col min="5" max="5" width="17.265625" customWidth="1"/>
-    <col min="7" max="7" width="20.1328125" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -462,19 +462,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>12.771000000000001</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="B2" s="1">
-        <f>A2*23.52/14.419</f>
-        <v>20.831813579305084</v>
+        <f>A2*415.38/12.0081</f>
+        <v>7.0566967297074461</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <f>C2*23.52/9.657</f>
+        <f>C2*415.38/12.0081</f>
         <v>0</v>
       </c>
       <c r="E2">
@@ -488,40 +488,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4.1820000000000004</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:B60" si="0">A3*23.52/14.419</f>
-        <v>6.8215992787294546</v>
+        <f t="shared" ref="B3:B66" si="0">A3*415.38/12.0081</f>
+        <v>11.89952781872236</v>
       </c>
       <c r="C3">
-        <v>6.4969999999999999</v>
+        <v>0.24099999999999999</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D60" si="1">C3*23.52/9.657</f>
-        <v>15.823696800248523</v>
+        <f t="shared" ref="D3:D66" si="1">C3*415.38/12.0081</f>
+        <v>8.3365878032328169</v>
       </c>
       <c r="E3" s="1">
         <f>B3*180/(PI()*D3)</f>
-        <v>24.700223540338921</v>
+        <v>81.783187354773105</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G60" si="2">E3</f>
-        <v>24.700223540338921</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+        <f t="shared" ref="G3:G66" si="2">E3</f>
+        <v>81.783187354773105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.879</v>
+        <v>0.111</v>
       </c>
       <c r="B4" s="1">
         <f t="shared" si="0"/>
-        <v>1.4338081697759899</v>
+        <v>3.839673220576111</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -541,40 +541,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>6.79</v>
+        <v>0.223</v>
       </c>
       <c r="B5" s="1">
         <f t="shared" si="0"/>
-        <v>11.07571953672238</v>
+        <v>7.7139380917880427</v>
       </c>
       <c r="C5">
-        <v>6.2320000000000002</v>
+        <v>0.251</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="1"/>
-        <v>15.178278968623795</v>
+        <v>8.6825043095910246</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" ref="E5:E59" si="3">B5*180/(PI()*D5)</f>
-        <v>41.809218676017117</v>
+        <f t="shared" ref="E5:E68" si="3">B5*180/(PI()*D5)</f>
+        <v>50.904218451861986</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="2"/>
-        <v>41.809218676017117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+        <v>50.904218451861986</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>29.306000000000001</v>
+        <v>0.35599999999999998</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" si="0"/>
-        <v>47.803392745682778</v>
+        <v>12.314627626352213</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -594,40 +594,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>15.443</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
-        <v>25.190329426451211</v>
+        <v>15.773792689934295</v>
       </c>
       <c r="C7">
-        <v>14.329000000000001</v>
+        <v>0.47899999999999998</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="1"/>
-        <v>34.898838148493319</v>
+        <v>16.569400654558173</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="3"/>
-        <v>41.356665071159952</v>
+        <v>54.544625173205716</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="2"/>
-        <v>41.356665071159952</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+        <v>54.544625173205716</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4.2590000000000003</v>
+        <v>0.1046</v>
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
-        <v>6.9472002219293989</v>
+        <v>3.6182866565068577</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -647,40 +647,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2.5550000000000002</v>
+        <v>0.38650000000000001</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
-        <v>4.1676676607254315</v>
+        <v>13.369672970744748</v>
       </c>
       <c r="C9">
-        <v>3.056</v>
+        <v>0.35659999999999997</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="1"/>
-        <v>7.4430071450761108</v>
+        <v>12.335382616733703</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="3"/>
-        <v>32.082431565405422</v>
+        <v>62.09988441336602</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="2"/>
-        <v>32.082431565405422</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>62.09988441336602</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>0.95399999999999996</v>
+        <v>0.23849999999999999</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
-        <v>1.556146750814897</v>
+        <v>8.250108676643265</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -700,40 +700,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>3.9590000000000001</v>
+        <v>0.88929999999999998</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
-        <v>6.4578458977737707</v>
+        <v>30.762354910435452</v>
       </c>
       <c r="C11">
-        <v>2.2160000000000002</v>
+        <v>0.35809999999999997</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="1"/>
-        <v>5.397154395775086</v>
+        <v>12.387270092687434</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="3"/>
-        <v>68.555999616752175</v>
+        <v>142.28745244619972</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="2"/>
-        <v>68.555999616752175</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>142.28745244619972</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>0.96399999999999997</v>
+        <v>0.15359999999999999</v>
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
-        <v>1.5724585616200843</v>
+        <v>5.3132775376620769</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -753,40 +753,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>4.298</v>
+        <v>0.41299999999999998</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
-        <v>7.0108162840696302</v>
+        <v>14.286351712593998</v>
       </c>
       <c r="C13">
-        <v>2.9049999999999998</v>
+        <v>0.247</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="1"/>
-        <v>7.0752407579993779</v>
+        <v>8.5441377070477422</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="3"/>
-        <v>56.774065753822363</v>
+        <v>95.802254813372471</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="2"/>
-        <v>56.774065753822363</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+        <v>95.802254813372471</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>0.80600000000000005</v>
+        <v>0.2225</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
-        <v>1.3147319508981206</v>
+        <v>7.6966422664701319</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -806,40 +806,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1.8360000000000001</v>
+        <v>0.16869999999999999</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
-        <v>2.9948484638324433</v>
+        <v>5.8356114622629711</v>
       </c>
       <c r="C15">
-        <v>1.599</v>
+        <v>8.1299999999999997E-2</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="1"/>
-        <v>3.894426840633737</v>
+        <v>2.8123011966922324</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="3"/>
-        <v>44.060957948542153</v>
+        <v>118.89050435248446</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="2"/>
-        <v>44.060957948542153</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+        <v>118.89050435248446</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>28.831</v>
+        <v>0.20519999999999999</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
-        <v>47.028581732436365</v>
+        <v>7.0982067104704312</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -859,40 +859,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>28.702999999999999</v>
+        <v>0.28120000000000001</v>
       </c>
       <c r="B17" s="1">
         <f t="shared" si="0"/>
-        <v>46.819790554129966</v>
+        <v>9.7271721587928148</v>
       </c>
       <c r="C17">
-        <v>20.260000000000002</v>
+        <v>0.16089999999999999</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="1"/>
-        <v>49.344019881950921</v>
+        <v>5.5657965873035691</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="3"/>
-        <v>54.364772121441192</v>
+        <v>100.13407830378344</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="2"/>
-        <v>54.364772121441192</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+        <v>100.13407830378344</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>3.4540000000000002</v>
+        <v>0.13450000000000001</v>
       </c>
       <c r="B18" s="1">
         <f t="shared" si="0"/>
-        <v>5.6340994521117969</v>
+        <v>4.6525770105179003</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -912,40 +912,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>3.3159999999999998</v>
+        <v>0.19170000000000001</v>
       </c>
       <c r="B19" s="1">
         <f t="shared" si="0"/>
-        <v>5.4089964630002072</v>
+        <v>6.6312194268868518</v>
       </c>
       <c r="C19">
-        <v>5.3929999999999998</v>
+        <v>0.1144</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" si="1"/>
-        <v>13.134861758310032</v>
+        <v>3.9572848327379018</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="3"/>
-        <v>23.594665435670048</v>
+        <v>96.010497663093375</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="2"/>
-        <v>23.594665435670048</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+        <v>96.010497663093375</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>0.91300000000000003</v>
+        <v>0.19209999999999999</v>
       </c>
       <c r="B20" s="1">
         <f t="shared" si="0"/>
-        <v>1.4892683265136279</v>
+        <v>6.6450560871411781</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -965,40 +965,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2.3530000000000002</v>
+        <v>0.28539999999999999</v>
       </c>
       <c r="B21" s="1">
         <f t="shared" si="0"/>
-        <v>3.8381690824606425</v>
+        <v>9.8724570914632608</v>
       </c>
       <c r="C21">
-        <v>2.988</v>
+        <v>0.14280000000000001</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" si="1"/>
-        <v>7.2773904939422183</v>
+        <v>4.9396877107952131</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="3"/>
-        <v>30.218371498087226</v>
+        <v>114.51131283637039</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="2"/>
-        <v>30.218371498087226</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+        <v>114.51131283637039</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>4.4809999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="B22" s="1">
         <f t="shared" si="0"/>
-        <v>7.3093224218045627</v>
+        <v>3.4591650635820823</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1018,40 +1018,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2.512</v>
+        <v>0.27589999999999998</v>
       </c>
       <c r="B23" s="1">
         <f t="shared" si="0"/>
-        <v>4.0975268742631252</v>
+        <v>9.543836410422962</v>
       </c>
       <c r="C23">
-        <v>2.964</v>
+        <v>0.1211</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" si="1"/>
-        <v>7.2189375582479025</v>
+        <v>4.189048891997901</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="3"/>
-        <v>32.521544125073483</v>
+        <v>130.53596670238986</v>
       </c>
       <c r="F23" s="1">
         <v>0</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" si="2"/>
-        <v>32.521544125073483</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+        <v>130.53596670238986</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>0.70199999999999996</v>
+        <v>0.3397</v>
       </c>
       <c r="B24" s="1">
         <f t="shared" si="0"/>
-        <v>1.1450891185241694</v>
+        <v>11.750783720988332</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1071,40 +1071,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>4.5309999999999997</v>
+        <v>0.41120000000000001</v>
       </c>
       <c r="B25" s="1">
         <f t="shared" si="0"/>
-        <v>7.3908814758304997</v>
+        <v>14.224086741449522</v>
       </c>
       <c r="C25" s="1">
-        <v>14.57</v>
+        <v>0.29770000000000002</v>
       </c>
       <c r="D25" s="1">
         <f t="shared" si="1"/>
-        <v>35.485803044423733</v>
+        <v>10.297934394283859</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="3"/>
-        <v>11.933400941113902</v>
+        <v>79.140156317700544</v>
       </c>
       <c r="F25" s="1">
         <v>0</v>
       </c>
       <c r="G25" s="1">
         <f t="shared" si="2"/>
-        <v>11.933400941113902</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
+        <v>79.140156317700544</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>26.416</v>
+        <v>0.1</v>
       </c>
       <c r="B26" s="1">
         <f t="shared" si="0"/>
-        <v>43.089279422983559</v>
+        <v>3.4591650635820823</v>
       </c>
       <c r="C26" s="1">
         <v>0</v>
@@ -1124,40 +1124,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>11.41</v>
+        <v>0.3599</v>
       </c>
       <c r="B27" s="1">
         <f t="shared" si="0"/>
-        <v>18.61177612871905</v>
+        <v>12.449535063831913</v>
       </c>
       <c r="C27" s="1">
-        <v>7.0019999999999998</v>
+        <v>0.37030000000000002</v>
       </c>
       <c r="D27" s="1">
         <f t="shared" si="1"/>
-        <v>17.0536439888164</v>
+        <v>12.80928823044445</v>
       </c>
       <c r="E27" s="1">
         <f t="shared" si="3"/>
-        <v>62.530695616564635</v>
+        <v>55.68660828182103</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
       </c>
       <c r="G27" s="1">
         <f t="shared" si="2"/>
-        <v>62.530695616564635</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
+        <v>55.68660828182103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>1.4139999999999999</v>
+        <v>0.1326</v>
       </c>
       <c r="B28" s="1">
         <f t="shared" si="0"/>
-        <v>2.3064900478535262</v>
+        <v>4.58685287430984</v>
       </c>
       <c r="C28" s="1">
         <v>0</v>
@@ -1177,40 +1177,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>6.5570000000000004</v>
+        <v>0.20180000000000001</v>
       </c>
       <c r="B29" s="1">
         <f t="shared" si="0"/>
-        <v>10.695654344961509</v>
+        <v>6.9805950983086413</v>
       </c>
       <c r="C29" s="1">
-        <v>7.0709999999999997</v>
+        <v>0.18490000000000001</v>
       </c>
       <c r="D29" s="1">
         <f t="shared" si="1"/>
-        <v>17.221696178937556</v>
+        <v>6.3959962025632695</v>
       </c>
       <c r="E29" s="1">
         <f t="shared" si="3"/>
-        <v>35.583942878201533</v>
+        <v>62.532657142996285</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
       </c>
       <c r="G29" s="1">
         <f t="shared" si="2"/>
-        <v>35.583942878201533</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
+        <v>62.532657142996285</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>8.3729999999999993</v>
+        <v>0.14080000000000001</v>
       </c>
       <c r="B30" s="1">
         <f t="shared" si="0"/>
-        <v>13.657879187183575</v>
+        <v>4.8705044095235719</v>
       </c>
       <c r="C30" s="1">
         <v>0</v>
@@ -1230,45 +1230,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>3.4540000000000002</v>
+        <v>0.39439999999999997</v>
       </c>
       <c r="B31" s="1">
         <f t="shared" si="0"/>
-        <v>5.6340994521117969</v>
+        <v>13.642947010767729</v>
       </c>
       <c r="C31" s="1">
-        <v>4.2370000000000001</v>
+        <v>0.36130000000000001</v>
       </c>
       <c r="D31" s="1">
         <f t="shared" si="1"/>
-        <v>10.319378689033861</v>
+        <v>12.497963374722062</v>
       </c>
       <c r="E31" s="1">
         <f t="shared" si="3"/>
-        <v>31.281933698781447</v>
+        <v>62.544853141322079</v>
       </c>
       <c r="F31" s="1">
         <v>0</v>
       </c>
       <c r="G31" s="1">
         <f t="shared" si="2"/>
-        <v>31.281933698781447</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+        <v>62.544853141322079</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>1.417</v>
+        <v>0.1938</v>
       </c>
       <c r="B32" s="1">
         <f t="shared" si="0"/>
-        <v>2.3113835910950828</v>
+        <v>6.7038618932220739</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1283,40 +1283,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>4.8840000000000003</v>
+        <v>0.27029999999999998</v>
       </c>
       <c r="B33" s="1">
         <f t="shared" si="0"/>
-        <v>7.9666883972536242</v>
+        <v>9.3501231668623657</v>
       </c>
       <c r="C33">
-        <v>12.837999999999999</v>
-      </c>
-      <c r="D33">
-        <f t="shared" si="1"/>
-        <v>31.267449518483996</v>
+        <v>0.54642000000000002</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="1"/>
+        <v>18.901569740425213</v>
       </c>
       <c r="E33" s="1">
         <f t="shared" si="3"/>
-        <v>14.598492326297238</v>
+        <v>28.342756858069155</v>
       </c>
       <c r="F33" s="1">
         <v>0</v>
       </c>
       <c r="G33" s="1">
         <f t="shared" si="2"/>
-        <v>14.598492326297238</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+        <v>28.342756858069155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>22.408000000000001</v>
+        <v>0.45250000000000001</v>
       </c>
       <c r="B34" s="1">
         <f t="shared" si="0"/>
-        <v>36.551505652264375</v>
+        <v>15.652721912708921</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1336,40 +1336,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>15.189</v>
+        <v>0.27789999999999998</v>
       </c>
       <c r="B35" s="1">
         <f t="shared" si="0"/>
-        <v>24.776009431999444</v>
+        <v>9.613019711694605</v>
       </c>
       <c r="C35">
-        <v>7.1239999999999997</v>
+        <v>0.2334</v>
       </c>
       <c r="D35" s="1">
         <f t="shared" si="1"/>
-        <v>17.350779745262503</v>
+        <v>8.0736912584005793</v>
       </c>
       <c r="E35" s="1">
         <f t="shared" si="3"/>
-        <v>81.815387808002598</v>
+        <v>68.219782033785677</v>
       </c>
       <c r="F35" s="1">
         <v>0</v>
       </c>
       <c r="G35" s="1">
         <f t="shared" si="2"/>
-        <v>81.815387808002598</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+        <v>68.219782033785677</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>16.594000000000001</v>
+        <v>7.2300000000000003E-2</v>
       </c>
       <c r="B36" s="1">
         <f t="shared" si="0"/>
-        <v>27.067818850128305</v>
+        <v>2.5009763409698453</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1389,40 +1389,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>15.951000000000001</v>
+        <v>0.2203</v>
       </c>
       <c r="B37" s="1">
         <f t="shared" si="0"/>
-        <v>26.018969415354743</v>
+        <v>7.6205406350713263</v>
       </c>
       <c r="C37">
-        <v>6.4660000000000002</v>
+        <v>0.21379999999999999</v>
       </c>
       <c r="D37" s="1">
         <f t="shared" si="1"/>
-        <v>15.748195091643368</v>
+        <v>7.3956949059384911</v>
       </c>
       <c r="E37" s="1">
         <f t="shared" si="3"/>
-        <v>94.663364665253894</v>
+        <v>59.037699844396798</v>
       </c>
       <c r="F37" s="1">
         <v>0</v>
       </c>
       <c r="G37" s="1">
         <f t="shared" si="2"/>
-        <v>94.663364665253894</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+        <v>59.037699844396798</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>11.147</v>
+        <v>0.61370000000000002</v>
       </c>
       <c r="B38" s="1">
         <f t="shared" si="0"/>
-        <v>18.182775504542615</v>
+        <v>21.228895995203239</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1442,40 +1442,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>10.766</v>
+        <v>0.17510000000000001</v>
       </c>
       <c r="B39" s="1">
         <f t="shared" si="0"/>
-        <v>17.561295512864969</v>
+        <v>6.0569980263322263</v>
       </c>
       <c r="C39">
-        <v>5.782</v>
+        <v>0.1928</v>
       </c>
       <c r="D39" s="1">
         <f t="shared" si="1"/>
-        <v>14.08228642435539</v>
+        <v>6.6692702425862533</v>
       </c>
       <c r="E39" s="1">
         <f t="shared" si="3"/>
-        <v>71.45062139405043</v>
+        <v>52.03574166359293</v>
       </c>
       <c r="F39" s="1">
         <v>0</v>
       </c>
       <c r="G39" s="1">
         <f t="shared" si="2"/>
-        <v>71.45062139405043</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+        <v>52.03574166359293</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>2.5049999999999999</v>
+        <v>9.4299999999999995E-2</v>
       </c>
       <c r="B40" s="1">
         <f t="shared" si="0"/>
-        <v>4.0861086066994927</v>
+        <v>3.2619926549579028</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1495,40 +1495,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>11.691000000000001</v>
+        <v>0.21809999999999999</v>
       </c>
       <c r="B41" s="1">
         <f t="shared" si="0"/>
-        <v>19.070138012344824</v>
+        <v>7.5444390036725197</v>
       </c>
       <c r="C41">
-        <v>11.118</v>
+        <v>0.33910000000000001</v>
       </c>
       <c r="D41" s="1">
         <f t="shared" si="1"/>
-        <v>27.078322460391426</v>
+        <v>11.73002873060684</v>
       </c>
       <c r="E41" s="1">
         <f t="shared" si="3"/>
-        <v>40.351038157463634</v>
+        <v>36.851104428791658</v>
       </c>
       <c r="F41" s="1">
         <v>0</v>
       </c>
       <c r="G41" s="1">
         <f t="shared" si="2"/>
-        <v>40.351038157463634</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+        <v>36.851104428791658</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>15.464</v>
+        <v>9.7600000000000006E-2</v>
       </c>
       <c r="B42" s="1">
         <f t="shared" si="0"/>
-        <v>25.224584229142103</v>
+        <v>3.3761451020561122</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -1548,40 +1548,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>14.564</v>
+        <v>0.25140000000000001</v>
       </c>
       <c r="B43" s="1">
         <f t="shared" si="0"/>
-        <v>23.756521256675217</v>
+        <v>8.6963409698453553</v>
       </c>
       <c r="C43">
-        <v>10.507</v>
+        <v>0.36730000000000002</v>
       </c>
       <c r="D43" s="1">
         <f t="shared" si="1"/>
-        <v>25.590208139173658</v>
+        <v>12.705513278536987</v>
       </c>
       <c r="E43" s="1">
         <f t="shared" si="3"/>
-        <v>53.19020449218862</v>
+        <v>39.216332615270616</v>
       </c>
       <c r="F43" s="1">
         <v>0</v>
       </c>
       <c r="G43" s="1">
         <f t="shared" si="2"/>
-        <v>53.19020449218862</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+        <v>39.216332615270616</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>14.09</v>
+        <v>5.8299999999999998E-2</v>
       </c>
       <c r="B44" s="1">
         <f t="shared" si="0"/>
-        <v>22.983341424509327</v>
+        <v>2.0166932320683535</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -1601,40 +1601,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>16.548999999999999</v>
+        <v>0.27689999999999998</v>
       </c>
       <c r="B45" s="1">
         <f t="shared" si="0"/>
-        <v>26.994415701504956</v>
+        <v>9.5784280610587853</v>
       </c>
       <c r="C45">
-        <v>9.4879999999999995</v>
+        <v>0.55679999999999996</v>
       </c>
       <c r="D45" s="1">
         <f t="shared" si="1"/>
-        <v>23.108393911152532</v>
+        <v>19.260631074025031</v>
       </c>
       <c r="E45" s="1">
         <f t="shared" si="3"/>
-        <v>66.930921121760264</v>
+        <v>28.493536902249456</v>
       </c>
       <c r="F45" s="1">
         <v>0</v>
       </c>
       <c r="G45" s="1">
         <f t="shared" si="2"/>
-        <v>66.930921121760264</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+        <v>28.493536902249456</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>2.831</v>
+        <v>2.3144999999999998</v>
       </c>
       <c r="B46" s="1">
         <f t="shared" si="0"/>
-        <v>4.6178736389486099</v>
+        <v>80.06237539660728</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -1654,40 +1654,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>16.62</v>
+        <v>0.3755</v>
       </c>
       <c r="B47" s="1">
         <f t="shared" si="0"/>
-        <v>27.110229558221789</v>
+        <v>12.989164813750717</v>
       </c>
       <c r="C47">
-        <v>13.077</v>
+        <v>0.58050000000000002</v>
       </c>
       <c r="D47" s="1">
         <f t="shared" si="1"/>
-        <v>31.849543336439886</v>
+        <v>20.080453194093987</v>
       </c>
       <c r="E47" s="1">
         <f t="shared" si="3"/>
-        <v>48.769984514652364</v>
+        <v>37.062127833182444</v>
       </c>
       <c r="F47" s="1">
         <v>0</v>
       </c>
       <c r="G47" s="1">
         <f t="shared" si="2"/>
-        <v>48.769984514652364</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+        <v>37.062127833182444</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>9.1530000000000005</v>
+        <v>7.0599999999999996E-2</v>
       </c>
       <c r="B48" s="1">
         <f t="shared" si="0"/>
-        <v>14.93020042998821</v>
+        <v>2.4421705348889495</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -1707,40 +1707,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>17.111999999999998</v>
+        <v>0.40799999999999997</v>
       </c>
       <c r="B49" s="1">
         <f t="shared" si="0"/>
-        <v>27.912770649837018</v>
+        <v>14.113393459414892</v>
       </c>
       <c r="C49">
-        <v>17.119</v>
+        <v>0.1978</v>
       </c>
       <c r="D49" s="1">
         <f t="shared" si="1"/>
-        <v>41.693991922957437</v>
+        <v>6.8422284957653581</v>
       </c>
       <c r="E49" s="1">
         <f t="shared" si="3"/>
-        <v>38.357659676901882</v>
+        <v>118.18340769129212</v>
       </c>
       <c r="F49">
         <v>0</v>
       </c>
       <c r="G49" s="1">
         <f t="shared" si="2"/>
-        <v>38.357659676901882</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+        <v>118.18340769129212</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>2.0619999999999998</v>
+        <v>0.08</v>
       </c>
       <c r="B50" s="1">
         <f t="shared" si="0"/>
-        <v>3.3634953880296825</v>
+        <v>2.7673320508656656</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -1760,40 +1760,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>4.4329999999999998</v>
+        <v>0.16089999999999999</v>
       </c>
       <c r="B51" s="1">
         <f t="shared" si="0"/>
-        <v>7.2310257299396623</v>
+        <v>5.5657965873035691</v>
       </c>
       <c r="C51">
-        <v>5.0529999999999999</v>
+        <v>0.25</v>
       </c>
       <c r="D51" s="1">
         <f t="shared" si="1"/>
-        <v>12.30677850264057</v>
+        <v>8.6479126589552049</v>
       </c>
       <c r="E51" s="1">
         <f t="shared" si="3"/>
-        <v>33.664964051083992</v>
+        <v>36.875563694619778</v>
       </c>
       <c r="F51" s="1">
         <v>0</v>
       </c>
       <c r="G51" s="1">
         <f t="shared" si="2"/>
-        <v>33.664964051083992</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+        <v>36.875563694619778</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>1.0680000000000001</v>
+        <v>0.122</v>
       </c>
       <c r="B52" s="1">
         <f t="shared" si="0"/>
-        <v>1.7421013939940355</v>
+        <v>4.2201813775701398</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -1813,40 +1813,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>15.894</v>
+        <v>1.1725000000000001</v>
       </c>
       <c r="B53" s="1">
         <f t="shared" si="0"/>
-        <v>25.925992093765171</v>
+        <v>40.558710370499917</v>
       </c>
       <c r="C53">
-        <v>5.806</v>
+        <v>0.90759999999999996</v>
       </c>
       <c r="D53" s="1">
         <f t="shared" si="1"/>
-        <v>14.140739360049704</v>
+        <v>31.395382117070973</v>
       </c>
       <c r="E53" s="1">
         <f t="shared" si="3"/>
-        <v>105.04754304848906</v>
+        <v>74.018622167352405</v>
       </c>
       <c r="F53" s="1">
         <v>0</v>
       </c>
       <c r="G53" s="1">
         <f t="shared" si="2"/>
-        <v>105.04754304848906</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+        <v>74.018622167352405</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>3.2269999999999999</v>
+        <v>0.4758</v>
       </c>
       <c r="B54" s="1">
         <f t="shared" si="0"/>
-        <v>5.263821346834038</v>
+        <v>16.458707372523545</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -1866,40 +1866,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>6.2119999999999997</v>
+        <v>0.36220000000000002</v>
       </c>
       <c r="B55" s="1">
         <f t="shared" si="0"/>
-        <v>10.132896872182535</v>
+        <v>12.529095860294301</v>
       </c>
       <c r="C55">
-        <v>3.99</v>
+        <v>0.25519999999999998</v>
       </c>
       <c r="D55" s="1">
         <f t="shared" si="1"/>
-        <v>9.7178005591798708</v>
+        <v>8.8277892422614723</v>
       </c>
       <c r="E55" s="1">
         <f t="shared" si="3"/>
-        <v>59.743171459609492</v>
+        <v>81.318696471937386</v>
       </c>
       <c r="F55" s="1">
         <v>0</v>
       </c>
       <c r="G55" s="1">
         <f t="shared" si="2"/>
-        <v>59.743171459609492</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+        <v>81.318696471937386</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>1.0820000000000001</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="B56" s="1">
         <f t="shared" si="0"/>
-        <v>1.7649379291212983</v>
+        <v>3.3553901116746196</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -1919,40 +1919,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>4.0970000000000004</v>
+        <v>0.23569999999999999</v>
       </c>
       <c r="B57" s="1">
         <f t="shared" si="0"/>
-        <v>6.6829488868853595</v>
+        <v>8.1532520548629659</v>
       </c>
       <c r="C57">
-        <v>3.3140000000000001</v>
-      </c>
-      <c r="D57">
-        <f t="shared" si="1"/>
-        <v>8.0713762037899972</v>
+        <v>0.30840000000000001</v>
+      </c>
+      <c r="D57" s="1">
+        <f t="shared" si="1"/>
+        <v>10.668065056087141</v>
       </c>
       <c r="E57">
         <f t="shared" si="3"/>
-        <v>47.43983631197684</v>
+        <v>43.789284147968552</v>
       </c>
       <c r="F57" s="1">
         <v>0</v>
       </c>
       <c r="G57" s="1">
         <f t="shared" si="2"/>
-        <v>47.43983631197684</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+        <v>43.789284147968552</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>1.546</v>
+        <v>0.73060000000000003</v>
       </c>
       <c r="B58" s="1">
         <f t="shared" si="0"/>
-        <v>2.5218059504820025</v>
+        <v>25.272659954530692</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -1972,40 +1972,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>6.681</v>
+        <v>0.58530000000000004</v>
       </c>
       <c r="B59" s="1">
         <f t="shared" si="0"/>
-        <v>10.897920798945835</v>
+        <v>20.246493117145924</v>
       </c>
       <c r="C59">
-        <v>7.4409999999999998</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="D59" s="1">
         <f t="shared" si="1"/>
-        <v>18.122845604224914</v>
+        <v>33.7268593699253</v>
       </c>
       <c r="E59" s="1">
         <f t="shared" si="3"/>
-        <v>34.454019025680452</v>
+        <v>34.395097178468802</v>
       </c>
       <c r="F59" s="1">
         <v>0</v>
       </c>
       <c r="G59" s="1">
         <f t="shared" si="2"/>
-        <v>34.454019025680452</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+        <v>34.395097178468802</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>6.3460000000000001</v>
+        <v>0.13869999999999999</v>
       </c>
       <c r="B60" s="1">
         <f t="shared" si="0"/>
-        <v>10.351475136972052</v>
+        <v>4.7978619431883471</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -2014,7 +2014,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E60">
+      <c r="E60" s="1">
         <v>0</v>
       </c>
       <c r="F60" s="1">
@@ -2022,6 +2022,1259 @@
       </c>
       <c r="G60" s="1">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>0.4249</v>
+      </c>
+      <c r="B61" s="1">
+        <f t="shared" si="0"/>
+        <v>14.697992355160265</v>
+      </c>
+      <c r="C61">
+        <v>0.4919</v>
+      </c>
+      <c r="D61" s="1">
+        <f t="shared" si="1"/>
+        <v>17.01563294776026</v>
+      </c>
+      <c r="E61" s="1">
+        <f t="shared" si="3"/>
+        <v>49.491719282595405</v>
+      </c>
+      <c r="F61" s="1">
+        <v>0</v>
+      </c>
+      <c r="G61" s="1">
+        <f t="shared" si="2"/>
+        <v>49.491719282595405</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>0.10780000000000001</v>
+      </c>
+      <c r="B62" s="1">
+        <f t="shared" si="0"/>
+        <v>3.7289799385414848</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E62" s="1">
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <v>0</v>
+      </c>
+      <c r="G62" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>0.42859999999999998</v>
+      </c>
+      <c r="B63" s="1">
+        <f t="shared" si="0"/>
+        <v>14.825981462512804</v>
+      </c>
+      <c r="C63">
+        <v>0.34489999999999998</v>
+      </c>
+      <c r="D63" s="1">
+        <f t="shared" si="1"/>
+        <v>11.9306603042946</v>
+      </c>
+      <c r="E63" s="1">
+        <f t="shared" si="3"/>
+        <v>71.200264132522719</v>
+      </c>
+      <c r="F63" s="1">
+        <v>0</v>
+      </c>
+      <c r="G63" s="1">
+        <f t="shared" si="2"/>
+        <v>71.200264132522719</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>7.6799999999999993E-2</v>
+      </c>
+      <c r="B64" s="1">
+        <f t="shared" si="0"/>
+        <v>2.6566387688310384</v>
+      </c>
+      <c r="D64" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E64" s="1">
+        <v>0</v>
+      </c>
+      <c r="F64" s="1">
+        <v>0</v>
+      </c>
+      <c r="G64" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>0.17380000000000001</v>
+      </c>
+      <c r="B65" s="1">
+        <f t="shared" si="0"/>
+        <v>6.0120288805056585</v>
+      </c>
+      <c r="C65">
+        <v>0.32690000000000002</v>
+      </c>
+      <c r="D65" s="1">
+        <f t="shared" si="1"/>
+        <v>11.308010592849826</v>
+      </c>
+      <c r="E65" s="1">
+        <f t="shared" si="3"/>
+        <v>30.461934779362828</v>
+      </c>
+      <c r="F65" s="1">
+        <v>0</v>
+      </c>
+      <c r="G65" s="1">
+        <f t="shared" si="2"/>
+        <v>30.461934779362828</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>0.26860000000000001</v>
+      </c>
+      <c r="B66" s="1">
+        <f t="shared" si="0"/>
+        <v>9.2913173607814716</v>
+      </c>
+      <c r="D66" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E66" s="1">
+        <v>0</v>
+      </c>
+      <c r="F66" s="1">
+        <v>0</v>
+      </c>
+      <c r="G66" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>0.66020000000000001</v>
+      </c>
+      <c r="B67" s="1">
+        <f t="shared" ref="B67:B110" si="4">A67*415.38/12.0081</f>
+        <v>22.837407749768907</v>
+      </c>
+      <c r="C67">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="D67" s="1">
+        <f t="shared" ref="D67:D110" si="5">C67*415.38/12.0081</f>
+        <v>26.704754290853671</v>
+      </c>
+      <c r="E67" s="1">
+        <f t="shared" si="3"/>
+        <v>48.998281910021966</v>
+      </c>
+      <c r="F67" s="1">
+        <v>0</v>
+      </c>
+      <c r="G67" s="1">
+        <f t="shared" ref="G67:G110" si="6">E67</f>
+        <v>48.998281910021966</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>0.43440000000000001</v>
+      </c>
+      <c r="B68" s="1">
+        <f t="shared" si="4"/>
+        <v>15.026613036200564</v>
+      </c>
+      <c r="D68" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E68" s="1">
+        <v>0</v>
+      </c>
+      <c r="F68" s="1">
+        <v>0</v>
+      </c>
+      <c r="G68" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>0.70550000000000002</v>
+      </c>
+      <c r="B69" s="1">
+        <f t="shared" si="4"/>
+        <v>24.404409523571587</v>
+      </c>
+      <c r="C69">
+        <v>0.54820000000000002</v>
+      </c>
+      <c r="D69" s="1">
+        <f t="shared" si="5"/>
+        <v>18.963142878556972</v>
+      </c>
+      <c r="E69" s="1">
+        <f t="shared" ref="E69:E110" si="7">B69*180/(PI()*D69)</f>
+        <v>73.736177392337794</v>
+      </c>
+      <c r="F69" s="1">
+        <v>0</v>
+      </c>
+      <c r="G69" s="1">
+        <f t="shared" si="6"/>
+        <v>73.736177392337794</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>0.15</v>
+      </c>
+      <c r="B70" s="1">
+        <f t="shared" si="4"/>
+        <v>5.1887475953731226</v>
+      </c>
+      <c r="D70" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E70" s="1">
+        <v>0</v>
+      </c>
+      <c r="F70" s="1">
+        <v>0</v>
+      </c>
+      <c r="G70" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>1.1671</v>
+      </c>
+      <c r="B71" s="1">
+        <f t="shared" si="4"/>
+        <v>40.371915457066478</v>
+      </c>
+      <c r="C71">
+        <v>1.4958</v>
+      </c>
+      <c r="D71" s="1">
+        <f t="shared" si="5"/>
+        <v>51.742191021060783</v>
+      </c>
+      <c r="E71" s="1">
+        <f t="shared" si="7"/>
+        <v>44.705110489181962</v>
+      </c>
+      <c r="F71" s="1">
+        <v>0</v>
+      </c>
+      <c r="G71" s="1">
+        <f t="shared" si="6"/>
+        <v>44.705110489181962</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>1.0061</v>
+      </c>
+      <c r="B72" s="1">
+        <f t="shared" si="4"/>
+        <v>34.802659704699323</v>
+      </c>
+      <c r="D72" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E72" s="1">
+        <v>0</v>
+      </c>
+      <c r="F72" s="1">
+        <v>0</v>
+      </c>
+      <c r="G72" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>0.24149999999999999</v>
+      </c>
+      <c r="B73" s="1">
+        <f t="shared" si="4"/>
+        <v>8.3538836285507276</v>
+      </c>
+      <c r="C73">
+        <v>0.34160000000000001</v>
+      </c>
+      <c r="D73" s="1">
+        <f t="shared" si="5"/>
+        <v>11.816507857196392</v>
+      </c>
+      <c r="E73" s="1">
+        <f t="shared" si="7"/>
+        <v>40.506237565601225</v>
+      </c>
+      <c r="F73" s="1">
+        <v>0</v>
+      </c>
+      <c r="G73" s="1">
+        <f t="shared" si="6"/>
+        <v>40.506237565601225</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>0.12859999999999999</v>
+      </c>
+      <c r="B74" s="1">
+        <f t="shared" si="4"/>
+        <v>4.4484862717665576</v>
+      </c>
+      <c r="D74" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E74" s="1">
+        <v>0</v>
+      </c>
+      <c r="F74" s="1">
+        <v>0</v>
+      </c>
+      <c r="G74" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>0.2417</v>
+      </c>
+      <c r="B75" s="1">
+        <f t="shared" si="4"/>
+        <v>8.3608019586778912</v>
+      </c>
+      <c r="C75">
+        <v>0.15659999999999999</v>
+      </c>
+      <c r="D75" s="1">
+        <f t="shared" si="5"/>
+        <v>5.4170524895695404</v>
+      </c>
+      <c r="E75" s="1">
+        <f t="shared" si="7"/>
+        <v>88.431608609910583</v>
+      </c>
+      <c r="F75" s="1">
+        <v>0</v>
+      </c>
+      <c r="G75" s="1">
+        <f t="shared" si="6"/>
+        <v>88.431608609910583</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>0.1221</v>
+      </c>
+      <c r="B76" s="1">
+        <f t="shared" si="4"/>
+        <v>4.2236405426337216</v>
+      </c>
+      <c r="D76" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E76" s="1">
+        <v>0</v>
+      </c>
+      <c r="F76" s="1">
+        <v>0</v>
+      </c>
+      <c r="G76" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>0.3377</v>
+      </c>
+      <c r="B77" s="1">
+        <f t="shared" si="4"/>
+        <v>11.681600419716689</v>
+      </c>
+      <c r="C77">
+        <v>0.22140000000000001</v>
+      </c>
+      <c r="D77" s="1">
+        <f t="shared" si="5"/>
+        <v>7.6585914507707304</v>
+      </c>
+      <c r="E77" s="1">
+        <f t="shared" si="7"/>
+        <v>87.392885011598452</v>
+      </c>
+      <c r="F77" s="1">
+        <v>0</v>
+      </c>
+      <c r="G77" s="1">
+        <f t="shared" si="6"/>
+        <v>87.392885011598452</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>0.123</v>
+      </c>
+      <c r="B78" s="1">
+        <f t="shared" si="4"/>
+        <v>4.2547730282059613</v>
+      </c>
+      <c r="D78" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E78" s="1">
+        <v>0</v>
+      </c>
+      <c r="F78" s="1">
+        <v>0</v>
+      </c>
+      <c r="G78" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>0.18010000000000001</v>
+      </c>
+      <c r="B79" s="1">
+        <f t="shared" si="4"/>
+        <v>6.2299562795113301</v>
+      </c>
+      <c r="C79">
+        <v>0.1171</v>
+      </c>
+      <c r="D79" s="1">
+        <f t="shared" si="5"/>
+        <v>4.0506822894546177</v>
+      </c>
+      <c r="E79" s="1">
+        <f t="shared" si="7"/>
+        <v>88.121006748984868</v>
+      </c>
+      <c r="F79" s="1">
+        <v>0</v>
+      </c>
+      <c r="G79" s="1">
+        <f t="shared" si="6"/>
+        <v>88.121006748984868</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>0.1033</v>
+      </c>
+      <c r="B80" s="1">
+        <f t="shared" si="4"/>
+        <v>3.5733175106802908</v>
+      </c>
+      <c r="D80" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E80" s="1">
+        <v>0</v>
+      </c>
+      <c r="F80" s="1">
+        <v>0</v>
+      </c>
+      <c r="G80" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>0.29809999999999998</v>
+      </c>
+      <c r="B81" s="1">
+        <f t="shared" si="4"/>
+        <v>10.311771054538186</v>
+      </c>
+      <c r="C81">
+        <v>0.1449</v>
+      </c>
+      <c r="D81" s="1">
+        <f t="shared" si="5"/>
+        <v>5.012330177130436</v>
+      </c>
+      <c r="E81" s="1">
+        <f t="shared" si="7"/>
+        <v>117.87351188992299</v>
+      </c>
+      <c r="F81" s="1">
+        <v>0</v>
+      </c>
+      <c r="G81" s="1">
+        <f t="shared" si="6"/>
+        <v>117.87351188992299</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>0.1017</v>
+      </c>
+      <c r="B82" s="1">
+        <f t="shared" si="4"/>
+        <v>3.5179708696629772</v>
+      </c>
+      <c r="D82" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E82" s="1">
+        <v>0</v>
+      </c>
+      <c r="F82" s="1">
+        <v>0</v>
+      </c>
+      <c r="G82" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>0.2339</v>
+      </c>
+      <c r="B83" s="1">
+        <f t="shared" si="4"/>
+        <v>8.0909870837184901</v>
+      </c>
+      <c r="C83">
+        <v>0.1212</v>
+      </c>
+      <c r="D83" s="1">
+        <f t="shared" si="5"/>
+        <v>4.1925080570614837</v>
+      </c>
+      <c r="E83" s="1">
+        <f t="shared" si="7"/>
+        <v>110.57329066097323</v>
+      </c>
+      <c r="F83" s="1">
+        <v>0</v>
+      </c>
+      <c r="G83" s="1">
+        <f t="shared" si="6"/>
+        <v>110.57329066097323</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>9.4299999999999995E-2</v>
+      </c>
+      <c r="B84" s="1">
+        <f t="shared" si="4"/>
+        <v>3.2619926549579028</v>
+      </c>
+      <c r="D84" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E84" s="1">
+        <v>0</v>
+      </c>
+      <c r="F84" s="1">
+        <v>0</v>
+      </c>
+      <c r="G84" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>0.17080000000000001</v>
+      </c>
+      <c r="B85" s="1">
+        <f t="shared" si="4"/>
+        <v>5.9082539285981959</v>
+      </c>
+      <c r="C85">
+        <v>0.19819999999999999</v>
+      </c>
+      <c r="D85" s="1">
+        <f t="shared" si="5"/>
+        <v>6.8560651560196852</v>
+      </c>
+      <c r="E85" s="1">
+        <f t="shared" si="7"/>
+        <v>49.374970438115341</v>
+      </c>
+      <c r="F85" s="1">
+        <v>0</v>
+      </c>
+      <c r="G85" s="1">
+        <f t="shared" si="6"/>
+        <v>49.374970438115341</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>0.17030000000000001</v>
+      </c>
+      <c r="B86" s="1">
+        <f t="shared" si="4"/>
+        <v>5.890958103280286</v>
+      </c>
+      <c r="D86" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E86" s="1">
+        <v>0</v>
+      </c>
+      <c r="F86" s="1">
+        <v>0</v>
+      </c>
+      <c r="G86" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>0.33169999999999999</v>
+      </c>
+      <c r="B87" s="1">
+        <f t="shared" si="4"/>
+        <v>11.474050515901766</v>
+      </c>
+      <c r="C87">
+        <v>0.60509999999999997</v>
+      </c>
+      <c r="D87" s="1">
+        <f t="shared" si="5"/>
+        <v>20.931407799735176</v>
+      </c>
+      <c r="E87" s="1">
+        <f t="shared" si="7"/>
+        <v>31.408048363062978</v>
+      </c>
+      <c r="F87" s="1">
+        <v>0</v>
+      </c>
+      <c r="G87" s="1">
+        <f t="shared" si="6"/>
+        <v>31.408048363062978</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>0.37</v>
+      </c>
+      <c r="B88" s="1">
+        <f t="shared" si="4"/>
+        <v>12.798910735253703</v>
+      </c>
+      <c r="D88" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E88" s="1">
+        <v>0</v>
+      </c>
+      <c r="F88" s="1">
+        <v>0</v>
+      </c>
+      <c r="G88" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>0.28060000000000002</v>
+      </c>
+      <c r="B89" s="1">
+        <f t="shared" si="4"/>
+        <v>9.7064171684113223</v>
+      </c>
+      <c r="C89">
+        <v>0.42470000000000002</v>
+      </c>
+      <c r="D89" s="1">
+        <f t="shared" si="5"/>
+        <v>14.691074025033103</v>
+      </c>
+      <c r="E89" s="1">
+        <f t="shared" si="7"/>
+        <v>37.855417309561808</v>
+      </c>
+      <c r="F89" s="1">
+        <v>0</v>
+      </c>
+      <c r="G89" s="1">
+        <f t="shared" si="6"/>
+        <v>37.855417309561808</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>7.8600000000000003E-2</v>
+      </c>
+      <c r="B90" s="1">
+        <f t="shared" si="4"/>
+        <v>2.7189037399755165</v>
+      </c>
+      <c r="D90" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E90" s="1">
+        <v>0</v>
+      </c>
+      <c r="F90" s="1">
+        <v>0</v>
+      </c>
+      <c r="G90" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>0.2316</v>
+      </c>
+      <c r="B91" s="1">
+        <f t="shared" si="4"/>
+        <v>8.0114262872561017</v>
+      </c>
+      <c r="C91">
+        <v>0.4042</v>
+      </c>
+      <c r="D91" s="1">
+        <f t="shared" si="5"/>
+        <v>13.981945186998773</v>
+      </c>
+      <c r="E91" s="1">
+        <f t="shared" si="7"/>
+        <v>32.82954610398285</v>
+      </c>
+      <c r="F91" s="1">
+        <v>0</v>
+      </c>
+      <c r="G91" s="1">
+        <f t="shared" si="6"/>
+        <v>32.82954610398285</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>4.4699999999999997E-2</v>
+      </c>
+      <c r="B92" s="1">
+        <f t="shared" si="4"/>
+        <v>1.5462467834211906</v>
+      </c>
+      <c r="D92" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E92" s="1">
+        <v>0</v>
+      </c>
+      <c r="F92" s="1">
+        <v>0</v>
+      </c>
+      <c r="G92" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>0.1336</v>
+      </c>
+      <c r="B93" s="1">
+        <f t="shared" si="4"/>
+        <v>4.6214445249456615</v>
+      </c>
+      <c r="C93">
+        <v>0.15290000000000001</v>
+      </c>
+      <c r="D93" s="1">
+        <f t="shared" si="5"/>
+        <v>5.2890633822170035</v>
+      </c>
+      <c r="E93" s="1">
+        <f t="shared" si="7"/>
+        <v>50.063545735433607</v>
+      </c>
+      <c r="F93" s="1">
+        <v>0</v>
+      </c>
+      <c r="G93" s="1">
+        <f t="shared" si="6"/>
+        <v>50.063545735433607</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>0.53039999999999998</v>
+      </c>
+      <c r="B94" s="1">
+        <f t="shared" si="4"/>
+        <v>18.34741149723936</v>
+      </c>
+      <c r="D94" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E94" s="1">
+        <v>0</v>
+      </c>
+      <c r="F94" s="1">
+        <v>0</v>
+      </c>
+      <c r="G94" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>1.1011500000000001</v>
+      </c>
+      <c r="B95" s="1">
+        <f t="shared" si="4"/>
+        <v>38.090596097634098</v>
+      </c>
+      <c r="C95">
+        <v>1.4648000000000001</v>
+      </c>
+      <c r="D95" s="1">
+        <f t="shared" si="5"/>
+        <v>50.669849851350335</v>
+      </c>
+      <c r="E95" s="1">
+        <f t="shared" si="7"/>
+        <v>43.071578106793147</v>
+      </c>
+      <c r="F95" s="1">
+        <v>0</v>
+      </c>
+      <c r="G95" s="1">
+        <f t="shared" si="6"/>
+        <v>43.071578106793147</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>9.9600000000000001E-3</v>
+      </c>
+      <c r="B96" s="1">
+        <f t="shared" si="4"/>
+        <v>0.34453284033277537</v>
+      </c>
+      <c r="D96" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E96" s="1">
+        <v>0</v>
+      </c>
+      <c r="F96" s="1">
+        <v>0</v>
+      </c>
+      <c r="G96" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>0.34370000000000001</v>
+      </c>
+      <c r="B97" s="1">
+        <f t="shared" si="4"/>
+        <v>11.889150323531616</v>
+      </c>
+      <c r="C97">
+        <v>0.1948</v>
+      </c>
+      <c r="D97" s="1">
+        <f t="shared" si="5"/>
+        <v>6.7384535438578954</v>
+      </c>
+      <c r="E97" s="1">
+        <f t="shared" si="7"/>
+        <v>101.09116744685009</v>
+      </c>
+      <c r="F97" s="1">
+        <v>0</v>
+      </c>
+      <c r="G97" s="1">
+        <f t="shared" si="6"/>
+        <v>101.09116744685009</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>0.1</v>
+      </c>
+      <c r="B98" s="1">
+        <f t="shared" si="4"/>
+        <v>3.4591650635820823</v>
+      </c>
+      <c r="D98" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E98" s="1">
+        <v>0</v>
+      </c>
+      <c r="F98" s="1">
+        <v>0</v>
+      </c>
+      <c r="G98" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>0.62202999999999997</v>
+      </c>
+      <c r="B99" s="1">
+        <f t="shared" si="4"/>
+        <v>21.517044444999623</v>
+      </c>
+      <c r="C99">
+        <v>0.47370000000000001</v>
+      </c>
+      <c r="D99" s="1">
+        <f t="shared" si="5"/>
+        <v>16.38606490618832</v>
+      </c>
+      <c r="E99" s="1">
+        <f t="shared" si="7"/>
+        <v>75.236845536252062</v>
+      </c>
+      <c r="F99" s="1">
+        <v>0</v>
+      </c>
+      <c r="G99" s="1">
+        <f t="shared" si="6"/>
+        <v>75.236845536252062</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>0.36649999999999999</v>
+      </c>
+      <c r="B100" s="1">
+        <f t="shared" si="4"/>
+        <v>12.677839958028331</v>
+      </c>
+      <c r="D100" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E100" s="1">
+        <v>0</v>
+      </c>
+      <c r="F100" s="1">
+        <v>0</v>
+      </c>
+      <c r="G100" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>0.25559999999999999</v>
+      </c>
+      <c r="B101" s="1">
+        <f t="shared" si="4"/>
+        <v>8.8416259025158013</v>
+      </c>
+      <c r="C101">
+        <v>0.31740000000000002</v>
+      </c>
+      <c r="D101" s="1">
+        <f t="shared" si="5"/>
+        <v>10.979389911809529</v>
+      </c>
+      <c r="E101" s="1">
+        <f t="shared" si="7"/>
+        <v>46.13989049635741</v>
+      </c>
+      <c r="F101" s="1">
+        <v>0</v>
+      </c>
+      <c r="G101" s="1">
+        <f t="shared" si="6"/>
+        <v>46.13989049635741</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>8.0600000000000005E-2</v>
+      </c>
+      <c r="B102" s="1">
+        <f t="shared" si="4"/>
+        <v>2.7880870412471577</v>
+      </c>
+      <c r="D102" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E102" s="1">
+        <v>0</v>
+      </c>
+      <c r="F102" s="1">
+        <v>0</v>
+      </c>
+      <c r="G102" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>0.43980000000000002</v>
+      </c>
+      <c r="B103" s="1">
+        <f t="shared" si="4"/>
+        <v>15.213407949633996</v>
+      </c>
+      <c r="C103">
+        <v>0.20910000000000001</v>
+      </c>
+      <c r="D103" s="1">
+        <f t="shared" si="5"/>
+        <v>7.2331141479501335</v>
+      </c>
+      <c r="E103" s="1">
+        <f t="shared" si="7"/>
+        <v>120.51020482952465</v>
+      </c>
+      <c r="F103" s="1">
+        <v>0</v>
+      </c>
+      <c r="G103" s="1">
+        <f t="shared" si="6"/>
+        <v>120.51020482952465</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>0.15909999999999999</v>
+      </c>
+      <c r="B104" s="1">
+        <f t="shared" si="4"/>
+        <v>5.5035316161590924</v>
+      </c>
+      <c r="D104" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E104" s="1">
+        <v>0</v>
+      </c>
+      <c r="F104" s="1">
+        <v>0</v>
+      </c>
+      <c r="G104" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>0.68569999999999998</v>
+      </c>
+      <c r="B105" s="1">
+        <f t="shared" si="4"/>
+        <v>23.719494840982332</v>
+      </c>
+      <c r="C105">
+        <v>0.54220000000000002</v>
+      </c>
+      <c r="D105" s="1">
+        <f t="shared" si="5"/>
+        <v>18.755592974742051</v>
+      </c>
+      <c r="E105" s="1">
+        <f t="shared" si="7"/>
+        <v>72.459822965917624</v>
+      </c>
+      <c r="F105" s="1">
+        <v>0</v>
+      </c>
+      <c r="G105" s="1">
+        <f t="shared" si="6"/>
+        <v>72.459822965917624</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>8.14E-2</v>
+      </c>
+      <c r="B106" s="1">
+        <f t="shared" si="4"/>
+        <v>2.8157603617558147</v>
+      </c>
+      <c r="D106" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E106" s="1">
+        <v>0</v>
+      </c>
+      <c r="F106" s="1">
+        <v>0</v>
+      </c>
+      <c r="G106" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>0.41410000000000002</v>
+      </c>
+      <c r="B107" s="1">
+        <f t="shared" si="4"/>
+        <v>14.324402528293401</v>
+      </c>
+      <c r="C107">
+        <v>0.21410000000000001</v>
+      </c>
+      <c r="D107" s="1">
+        <f t="shared" si="5"/>
+        <v>7.4060724011292383</v>
+      </c>
+      <c r="E107" s="1">
+        <f t="shared" si="7"/>
+        <v>110.81822651269214</v>
+      </c>
+      <c r="F107" s="1">
+        <v>0</v>
+      </c>
+      <c r="G107" s="1">
+        <f t="shared" si="6"/>
+        <v>110.81822651269214</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>0.25719999999999998</v>
+      </c>
+      <c r="B108" s="1">
+        <f t="shared" si="4"/>
+        <v>8.8969725435331153</v>
+      </c>
+      <c r="D108" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E108" s="1">
+        <v>0</v>
+      </c>
+      <c r="F108" s="1">
+        <v>0</v>
+      </c>
+      <c r="G108" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="B109" s="1">
+        <f t="shared" si="4"/>
+        <v>10.100761985659679</v>
+      </c>
+      <c r="C109">
+        <v>0.46589999999999998</v>
+      </c>
+      <c r="D109" s="1">
+        <f t="shared" si="5"/>
+        <v>16.116250031228919</v>
+      </c>
+      <c r="E109" s="1">
+        <f t="shared" si="7"/>
+        <v>35.909782394977547</v>
+      </c>
+      <c r="F109" s="1">
+        <v>0</v>
+      </c>
+      <c r="G109" s="1">
+        <f t="shared" si="6"/>
+        <v>35.909782394977547</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>0.33110000000000001</v>
+      </c>
+      <c r="B110" s="1">
+        <f t="shared" si="4"/>
+        <v>11.453295525520273</v>
+      </c>
+      <c r="D110" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E110" s="1">
+        <v>0</v>
+      </c>
+      <c r="F110" s="1">
+        <v>0</v>
+      </c>
+      <c r="G110" s="1">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>